<commit_message>
ppt 및 data 추가
</commit_message>
<xml_diff>
--- a/data/도로 및 배수로/시・도별_도로현황_20240704122613.xlsx
+++ b/data/도로 및 배수로/시・도별_도로현황_20240704122613.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace\Mini_Project3\data\도로 및 배수로\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace\backup_Local_Extinction\data\도로 및 배수로\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12255"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12255"/>
   </bookViews>
   <sheets>
     <sheet name="데이터" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="50">
   <si>
     <t>구분(1)</t>
   </si>
@@ -274,7 +274,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -295,13 +295,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -585,13 +586,13 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25:B26"/>
+      <selection activeCell="A14" sqref="A14:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -626,7 +627,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -661,7 +662,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -886,47 +887,58 @@
         <v>15</v>
       </c>
     </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B14" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15" s="11">
         <f>B4/$B10</f>
         <v>3829.9108714584841</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="11">
         <f t="shared" ref="C15:K15" si="0">C4/$B10</f>
         <v>3848.2165026775624</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15" s="11">
         <f t="shared" si="0"/>
         <v>3920.2679415198181</v>
       </c>
-      <c r="E15" s="12">
+      <c r="E15" s="11">
         <f t="shared" si="0"/>
         <v>3958.2856189893828</v>
       </c>
-      <c r="F15" s="12">
+      <c r="F15" s="11">
         <f t="shared" si="0"/>
         <v>3966.1052124446423</v>
       </c>
-      <c r="G15" s="12">
+      <c r="G15" s="11">
         <f t="shared" si="0"/>
         <v>3968.4881501658424</v>
       </c>
-      <c r="H15" s="12">
+      <c r="H15" s="11">
         <f t="shared" si="0"/>
         <v>3976.7135471677138</v>
       </c>
-      <c r="I15" s="12">
+      <c r="I15" s="11">
         <f t="shared" si="0"/>
         <v>4123.8831137547022</v>
       </c>
-      <c r="J15" s="12">
+      <c r="J15" s="11">
         <f t="shared" si="0"/>
         <v>4136.3851983619625</v>
       </c>
-      <c r="K15" s="12">
+      <c r="K15" s="11">
         <f t="shared" si="0"/>
         <v>4148.8761650638353</v>
       </c>
@@ -935,43 +947,43 @@
       <c r="A16" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="12">
+      <c r="B16" s="11">
         <f>B5/$B11</f>
         <v>859.76296997332872</v>
       </c>
-      <c r="C16" s="12">
+      <c r="C16" s="11">
         <f t="shared" ref="C16:K16" si="1">C5/$B11</f>
         <v>862.40858642347064</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D16" s="11">
         <f t="shared" si="1"/>
         <v>868.30207347500641</v>
       </c>
-      <c r="E16" s="12">
+      <c r="E16" s="11">
         <f t="shared" si="1"/>
         <v>865.61343887120358</v>
       </c>
-      <c r="F16" s="12">
+      <c r="F16" s="11">
         <f t="shared" si="1"/>
         <v>865.61343887120358</v>
       </c>
-      <c r="G16" s="12">
+      <c r="G16" s="11">
         <f t="shared" si="1"/>
         <v>866.68889271272474</v>
       </c>
-      <c r="H16" s="12">
+      <c r="H16" s="11">
         <f t="shared" si="1"/>
         <v>909.49195560526539</v>
       </c>
-      <c r="I16" s="12">
+      <c r="I16" s="11">
         <f t="shared" si="1"/>
         <v>909.49195560526539</v>
       </c>
-      <c r="J16" s="12">
+      <c r="J16" s="11">
         <f t="shared" si="1"/>
         <v>909.49195560526539</v>
       </c>
-      <c r="K16" s="12">
+      <c r="K16" s="11">
         <f t="shared" si="1"/>
         <v>909.49195560526539</v>
       </c>
@@ -980,43 +992,43 @@
       <c r="A17" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="12">
+      <c r="B17" s="11">
         <f>B6/$B12</f>
         <v>897.16740920750647</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C17" s="11">
         <f t="shared" ref="C17:K17" si="2">C6/$B12</f>
         <v>925.84177129742136</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17" s="11">
         <f t="shared" si="2"/>
         <v>927.55866072633989</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="11">
         <f t="shared" si="2"/>
         <v>930.37802079114351</v>
       </c>
-      <c r="F17" s="12">
+      <c r="F17" s="11">
         <f t="shared" si="2"/>
         <v>937.29863642500334</v>
       </c>
-      <c r="G17" s="12">
+      <c r="G17" s="11">
         <f t="shared" si="2"/>
         <v>935.47738625624413</v>
       </c>
-      <c r="H17" s="12">
+      <c r="H17" s="11">
         <f t="shared" si="2"/>
         <v>931.27285000675033</v>
       </c>
-      <c r="I17" s="12">
+      <c r="I17" s="11">
         <f t="shared" si="2"/>
         <v>933.5361144862967</v>
       </c>
-      <c r="J17" s="12">
+      <c r="J17" s="11">
         <f t="shared" si="2"/>
         <v>933.03078169299306</v>
       </c>
-      <c r="K17" s="12">
+      <c r="K17" s="11">
         <f t="shared" si="2"/>
         <v>937.70487376805727</v>
       </c>
@@ -1025,130 +1037,130 @@
       <c r="A18" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="12">
+      <c r="B18" s="11">
         <f>B7/$B13</f>
         <v>835.61042740224309</v>
       </c>
-      <c r="C18" s="12">
+      <c r="C18" s="11">
         <f t="shared" ref="C18:K18" si="3">C7/$B13</f>
         <v>860.34107305244015</v>
       </c>
-      <c r="D18" s="12">
+      <c r="D18" s="11">
         <f t="shared" si="3"/>
         <v>863.4993634434677</v>
       </c>
-      <c r="E18" s="12">
+      <c r="E18" s="11">
         <f t="shared" si="3"/>
         <v>877.13840557744766</v>
       </c>
-      <c r="F18" s="12">
+      <c r="F18" s="11">
         <f t="shared" si="3"/>
         <v>868.12391633828429</v>
       </c>
-      <c r="G18" s="12">
+      <c r="G18" s="11">
         <f t="shared" si="3"/>
         <v>869.05341012428005</v>
       </c>
-      <c r="H18" s="12">
+      <c r="H18" s="11">
         <f t="shared" si="3"/>
         <v>923.00648681418613</v>
       </c>
-      <c r="I18" s="12">
+      <c r="I18" s="11">
         <f t="shared" si="3"/>
         <v>919.98532888754164</v>
       </c>
-      <c r="J18" s="12">
+      <c r="J18" s="11">
         <f t="shared" si="3"/>
         <v>926.46911185207637</v>
       </c>
-      <c r="K18" s="12">
+      <c r="K18" s="11">
         <f t="shared" si="3"/>
         <v>939.95101545923012</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="12"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="12">
+      <c r="B22" s="11">
         <f>B17/$C12</f>
         <v>81.560673564318776</v>
       </c>
-      <c r="C22" s="12">
+      <c r="C22" s="11">
         <f t="shared" ref="C22:K22" si="4">C17/$C12</f>
         <v>84.167433754311034</v>
       </c>
-      <c r="D22" s="12">
+      <c r="D22" s="11">
         <f t="shared" si="4"/>
         <v>84.32351461148545</v>
       </c>
-      <c r="E22" s="12">
+      <c r="E22" s="11">
         <f t="shared" si="4"/>
         <v>84.579820071922143</v>
       </c>
-      <c r="F22" s="12">
+      <c r="F22" s="11">
         <f t="shared" si="4"/>
         <v>85.208966947727575</v>
       </c>
-      <c r="G22" s="12">
+      <c r="G22" s="11">
         <f t="shared" si="4"/>
         <v>85.043398750567647</v>
       </c>
-      <c r="H22" s="12">
+      <c r="H22" s="11">
         <f t="shared" si="4"/>
         <v>84.661168182431851</v>
       </c>
-      <c r="I22" s="12">
+      <c r="I22" s="11">
         <f t="shared" si="4"/>
         <v>84.866919498754243</v>
       </c>
-      <c r="J22" s="12">
+      <c r="J22" s="11">
         <f t="shared" si="4"/>
         <v>84.820980153908465</v>
       </c>
-      <c r="K22" s="12">
+      <c r="K22" s="11">
         <f t="shared" si="4"/>
         <v>85.24589761527794</v>
       </c>
@@ -1157,43 +1169,43 @@
       <c r="A23" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B23" s="12">
+      <c r="B23" s="11">
         <f>B18/$C13</f>
         <v>55.707361826816204</v>
       </c>
-      <c r="C23" s="12">
+      <c r="C23" s="11">
         <f t="shared" ref="C23:K23" si="5">C18/$C13</f>
         <v>57.35607153682934</v>
       </c>
-      <c r="D23" s="12">
+      <c r="D23" s="11">
         <f t="shared" si="5"/>
         <v>57.566624229564511</v>
       </c>
-      <c r="E23" s="12">
+      <c r="E23" s="11">
         <f t="shared" si="5"/>
         <v>58.47589370516318</v>
       </c>
-      <c r="F23" s="12">
+      <c r="F23" s="11">
         <f t="shared" si="5"/>
         <v>57.874927755885622</v>
       </c>
-      <c r="G23" s="12">
+      <c r="G23" s="11">
         <f t="shared" si="5"/>
         <v>57.936894008285336</v>
       </c>
-      <c r="H23" s="12">
+      <c r="H23" s="11">
         <f t="shared" si="5"/>
         <v>61.53376578761241</v>
       </c>
-      <c r="I23" s="12">
+      <c r="I23" s="11">
         <f t="shared" si="5"/>
         <v>61.332355259169439</v>
       </c>
-      <c r="J23" s="12">
+      <c r="J23" s="11">
         <f t="shared" si="5"/>
         <v>61.764607456805088</v>
       </c>
-      <c r="K23" s="12">
+      <c r="K23" s="11">
         <f t="shared" si="5"/>
         <v>62.66340103061534</v>
       </c>

</xml_diff>